<commit_message>
updated the census api work
</commit_message>
<xml_diff>
--- a/Data/Day4-Dictionaries/College-Majors/recent_Arts_edited.xlsx
+++ b/Data/Day4-Dictionaries/College-Majors/recent_Arts_edited.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Rank</t>
   </si>
@@ -79,6 +79,9 @@
     <t>Low_wage_jobs</t>
   </si>
   <si>
+    <t>Test_column</t>
+  </si>
+  <si>
     <t>Percent_Employed</t>
   </si>
   <si>
@@ -104,6 +107,9 @@
   </si>
   <si>
     <t>DRAMA AND THEATER ARTS</t>
+  </si>
+  <si>
+    <t>Arts</t>
   </si>
 </sst>
 </file>
@@ -461,13 +467,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,8 +540,11 @@
       <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:23">
       <c r="A2">
         <v>33</v>
       </c>
@@ -543,7 +552,10 @@
         <v>6099</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
       </c>
       <c r="E2">
         <v>3340</v>
@@ -596,11 +608,11 @@
       <c r="U2">
         <v>755</v>
       </c>
-      <c r="V2">
-        <v>0.872455089820359</v>
+      <c r="W2">
+        <v>0.8724550898203592</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:23">
       <c r="A3">
         <v>96</v>
       </c>
@@ -608,7 +620,10 @@
         <v>6004</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
       </c>
       <c r="E3">
         <v>103480</v>
@@ -661,11 +676,11 @@
       <c r="U3">
         <v>14839</v>
       </c>
-      <c r="V3">
-        <v>0.806754928488597</v>
+      <c r="W3">
+        <v>0.8067549284885969</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:23">
       <c r="A4">
         <v>142</v>
       </c>
@@ -673,7 +688,10 @@
         <v>6005</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
       </c>
       <c r="E4">
         <v>38761</v>
@@ -726,11 +744,11 @@
       <c r="U4">
         <v>5862</v>
       </c>
-      <c r="V4">
-        <v>0.810943990093135</v>
+      <c r="W4">
+        <v>0.8109439900931349</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:23">
       <c r="A5">
         <v>147</v>
       </c>
@@ -738,7 +756,10 @@
         <v>6002</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
       </c>
       <c r="E5">
         <v>60633</v>
@@ -791,11 +812,11 @@
       <c r="U5">
         <v>9286</v>
       </c>
-      <c r="V5">
-        <v>0.786073590289116</v>
+      <c r="W5">
+        <v>0.7860735902891165</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:23">
       <c r="A6">
         <v>150</v>
       </c>
@@ -803,7 +824,10 @@
         <v>6000</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
       </c>
       <c r="E6">
         <v>74440</v>
@@ -836,7 +860,7 @@
         <v>5486</v>
       </c>
       <c r="O6">
-        <v>0.084186296</v>
+        <v>0.08418629599999999</v>
       </c>
       <c r="P6">
         <v>30500</v>
@@ -856,11 +880,11 @@
       <c r="U6">
         <v>11880</v>
       </c>
-      <c r="V6">
-        <v>0.801706072004299</v>
+      <c r="W6">
+        <v>0.8017060720042988</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:23">
       <c r="A7">
         <v>154</v>
       </c>
@@ -868,7 +892,10 @@
         <v>6003</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
       </c>
       <c r="E7">
         <v>16250</v>
@@ -921,11 +948,11 @@
       <c r="U7">
         <v>2840</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>0.792</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:23">
       <c r="A8">
         <v>160</v>
       </c>
@@ -933,7 +960,10 @@
         <v>6007</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
       </c>
       <c r="E8">
         <v>16977</v>
@@ -966,7 +996,7 @@
         <v>1368</v>
       </c>
       <c r="O8">
-        <v>0.089552239</v>
+        <v>0.08955223900000001</v>
       </c>
       <c r="P8">
         <v>29000</v>
@@ -986,11 +1016,11 @@
       <c r="U8">
         <v>3586</v>
       </c>
-      <c r="V8">
-        <v>0.819226011662838</v>
+      <c r="W8">
+        <v>0.8192260116628379</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:23">
       <c r="A9">
         <v>167</v>
       </c>
@@ -998,7 +1028,10 @@
         <v>6001</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
       </c>
       <c r="E9">
         <v>43249</v>
@@ -1051,8 +1084,8 @@
       <c r="U9">
         <v>11068</v>
       </c>
-      <c r="V9">
-        <v>0.836204305301857</v>
+      <c r="W9">
+        <v>0.8362043053018567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>